<commit_message>
Fixed bug with removing commas within quotes
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheet outputs/parsed_collections.xlsx
+++ b/src/main/resources/spreadsheet outputs/parsed_collections.xlsx
@@ -865,7 +865,7 @@
     <t>Parma</t>
   </si>
   <si>
-    <t>”Bas”, A</t>
+    <t>”Bass”, A</t>
   </si>
   <si>
     <t>111|1115U1,D5|U1111|1</t>
@@ -922,7 +922,7 @@
     <t>Brunswick Tune</t>
   </si>
   <si>
-    <t>”Can”, Am</t>
+    <t>”Cant”, Am</t>
   </si>
   <si>
     <t>11234-3251</t>
@@ -937,7 +937,7 @@
     <t>Hymn 15th</t>
   </si>
   <si>
-    <t>att. “Milgrov”, 3 voices</t>
+    <t>att. “Milgrove”, 3 voices</t>
   </si>
   <si>
     <t>5|56-7|U13|2-1D7-6|5</t>
@@ -952,7 +952,7 @@
     <t>Rutland</t>
   </si>
   <si>
-    <t>“Rippon’s Coll.”, 3 voices</t>
+    <t>“Rippon’s Coll.n”, 3 voices</t>
   </si>
   <si>
     <t>5|U1-2-3-1D5-3|4-32|1</t>
@@ -970,7 +970,7 @@
     <t>Farndon</t>
   </si>
   <si>
-    <t>“Dr. Addington’s Colln”, 3 voices</t>
+    <t>“Dr. Addington’s Colln.”, 3 voices</t>
   </si>
   <si>
     <t>5|3-5-4-32-1|5U1-D7|6-U1-D7-65-4|3</t>
@@ -985,7 +985,7 @@
     <t>Cimbeline</t>
   </si>
   <si>
-    <t>att. “Dr Arn”, 3 voices</t>
+    <t>att. “Dr Arne”, 3 voices</t>
   </si>
   <si>
     <t>Dm</t>
@@ -1003,7 +1003,7 @@
     <t>Henley</t>
   </si>
   <si>
-    <t>att. “I. Smit”, 3 voices</t>
+    <t>att. “I. Smith”, 3 voices</t>
   </si>
   <si>
     <t>G</t>
@@ -1018,7 +1018,7 @@
     <t>Watchman</t>
   </si>
   <si>
-    <t>att. “Leac”, 4 voices</t>
+    <t>att. “Leach”, 4 voices</t>
   </si>
   <si>
     <t>E</t>
@@ -1102,7 +1102,7 @@
     <t>Chorus [from Handel’s Messiah]</t>
   </si>
   <si>
-    <t>“Bas”, D</t>
+    <t>“Bass”, D</t>
   </si>
   <si>
     <t>starts with upper voice: 1D765|654U111|4|1</t>

</xml_diff>